<commit_message>
sửa chức năng import student bằng excel
</commit_message>
<xml_diff>
--- a/storage/file/mau-them-sinh-vien.xlsx
+++ b/storage/file/mau-them-sinh-vien.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" calcOnSave="0"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Mẫu  thêm sinh viên</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Việt Nam</t>
   </si>
   <si>
-    <t>vvcau@gmail.com</t>
-  </si>
-  <si>
     <t>Nông nghiệp</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>0635175854</t>
   </si>
   <si>
-    <t>Kỹ thuật phần mềm K14c</t>
-  </si>
-  <si>
     <t>Thiết kế đồ hoạ</t>
   </si>
   <si>
@@ -166,22 +160,31 @@
     <t>DTC155D4845365458</t>
   </si>
   <si>
-    <t>DTC155D4801032442247</t>
-  </si>
-  <si>
-    <t>08550051224523524</t>
-  </si>
-  <si>
-    <t>0855441253542155453</t>
-  </si>
-  <si>
-    <t>0978512453244534</t>
-  </si>
-  <si>
-    <t>0369458125453453</t>
-  </si>
-  <si>
     <t>Số điện thoại mẹ</t>
+  </si>
+  <si>
+    <t>DTC155D4801030048</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
+  </si>
+  <si>
+    <t>0916854487</t>
+  </si>
+  <si>
+    <t>0369548757</t>
+  </si>
+  <si>
+    <t>085522485</t>
+  </si>
+  <si>
+    <t>085535125</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>vvc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -552,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +599,7 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -607,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -682,7 +685,7 @@
         <v>26</v>
       </c>
       <c r="AB3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="AC3" t="s">
         <v>27</v>
@@ -696,28 +699,28 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1">
         <v>35758</v>
       </c>
-      <c r="F4" s="4">
-        <v>1</v>
+      <c r="F4" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
         <v>42</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
@@ -732,10 +735,10 @@
         <v>30</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P4" t="s">
         <v>31</v>
@@ -747,16 +750,16 @@
         <v>30</v>
       </c>
       <c r="S4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" t="s">
         <v>32</v>
-      </c>
-      <c r="V4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -764,46 +767,46 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1">
         <v>35435</v>
       </c>
-      <c r="F5" s="4">
-        <v>1</v>
+      <c r="F5" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
         <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" t="s">
-        <v>46</v>
       </c>
       <c r="P5" t="s">
         <v>31</v>
@@ -815,13 +818,13 @@
         <v>30</v>
       </c>
       <c r="S5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>